<commit_message>
primo inserimento letture wallbox
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITLOAIT\Documents\GitHub\OrionLogger\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486967F2-AFD4-4D7F-98EE-A8ACE9FB2C7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0376E5B-C79B-45EB-81F7-90C28E4FBBA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strumenti" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Wattmeter" sheetId="2" r:id="rId4"/>
     <sheet name="Agilent" sheetId="3" r:id="rId5"/>
     <sheet name="Inverter" sheetId="4" r:id="rId6"/>
+    <sheet name="AC Station" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="191">
   <si>
     <t>ELENCO STRUMENTI</t>
   </si>
@@ -591,13 +592,34 @@
   <si>
     <t>[numero] + V/A se il livello è 
 in tensione o in corrente</t>
+  </si>
+  <si>
+    <t>PORTA</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>METER1 VL1</t>
+  </si>
+  <si>
+    <t>METER1 VL2</t>
+  </si>
+  <si>
+    <t>METER1 VL3</t>
+  </si>
+  <si>
+    <t>REGISTRO</t>
+  </si>
+  <si>
+    <t>502-RTU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -629,6 +651,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1303,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FCE3F72-A82B-43C8-A199-D908A3F357E6}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -2870,4 +2898,71 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073EBEDE-603A-4744-AA10-6C9743035A2C}">
+  <dimension ref="A1:AMJ4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11" style="13" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="1024" width="9.109375" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="C3" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="C4" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1626</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit dopo incontro Simone Martini
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -899,8 +899,6 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>10</t>
@@ -961,7 +959,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>abc</t>
+          <t>q1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -971,7 +969,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>300</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">

</xml_diff>

<commit_message>
Aggiunto il comando weiss in TestSeq
Adesso è possibile dare degli interi per settare la temperatura e l'umidità delle weiss
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="390" yWindow="390" windowWidth="13170" windowHeight="14025" tabRatio="600" firstSheet="2" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Colonnina" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bridge" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grafico" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Strumenti" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inverter" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Agilent" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Wattmeter" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Wattmeter2" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Colonnina" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Bridge" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Grafico" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Strumenti" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Inverter" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Agilent" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Wattmeter" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Wattmeter2" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>100000000000</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>

</xml_diff>